<commit_message>
updated asset_uid in cal sheets as per redmine $11481 and #11482
- added barcodes to legacy calibration sheets for CE04OSSM and CE06ISSM
as per redline #11481 and #11482

- converted from legacy sheets to new calibration and deployment sheets

- modified asset_uid to conform to new cgsn asset_uid schema

- ran replace_uid.csv to updated legacy asset_uid that were in older
deployment sheets. This also renames old cal sheets to the new asset_uid
</commit_message>
<xml_diff>
--- a/ARCHIVE/deployment/Omaha_Cal_Info_CE02SHSM_00004.xlsx
+++ b/ARCHIVE/deployment/Omaha_Cal_Info_CE02SHSM_00004.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaesm/Documents/dev/repos/ooi-integration/asset-management/ARCHIVE/deployment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaesm/Documents/dev/repos/najascutellatus/asset-management/ARCHIVE/deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="460" windowWidth="25600" windowHeight="28340" activeTab="1"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="50300" windowHeight="28340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -539,9 +539,6 @@
     <t>CGINS-MOPAKA-432260</t>
   </si>
   <si>
-    <t>CGINS-PCO2AA-00050</t>
-  </si>
-  <si>
     <t>CGINS-VELPTA-12703</t>
   </si>
   <si>
@@ -579,6 +576,9 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>CGINS-PCO2AA-25750</t>
   </si>
 </sst>
 </file>
@@ -2678,7 +2678,7 @@
   <dimension ref="A1:P119"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2770,7 +2770,7 @@
         <v>164</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G3" s="24" t="s">
         <v>21</v>
@@ -3287,7 +3287,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="80" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>136</v>
@@ -3337,7 +3337,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F22" s="67" t="s">
         <v>137</v>
@@ -3371,7 +3371,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F23" s="67" t="s">
         <v>137</v>
@@ -3423,10 +3423,10 @@
         <v>4</v>
       </c>
       <c r="E25" s="80" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="F25" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="G25" s="27" t="s">
         <v>25</v>
@@ -3457,10 +3457,10 @@
         <v>4</v>
       </c>
       <c r="E26" s="80" t="s">
+        <v>170</v>
+      </c>
+      <c r="F26" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="G26" s="27" t="s">
         <v>26</v>
@@ -3509,7 +3509,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="62" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F28" s="70" t="s">
         <v>138</v>
@@ -3545,7 +3545,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F29" s="71" t="s">
         <v>138</v>
@@ -3579,7 +3579,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F30" s="72" t="s">
         <v>138</v>
@@ -3613,7 +3613,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F31" s="73" t="s">
         <v>138</v>
@@ -3647,7 +3647,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F32" s="72" t="s">
         <v>138</v>
@@ -3681,7 +3681,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F33" s="73" t="s">
         <v>138</v>
@@ -3715,7 +3715,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F34" s="72" t="s">
         <v>138</v>
@@ -3767,7 +3767,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F36" s="67" t="s">
         <v>139</v>
@@ -3801,7 +3801,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F37" s="67" t="s">
         <v>139</v>
@@ -3835,7 +3835,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F38" s="67" t="s">
         <v>139</v>
@@ -3869,7 +3869,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F39" s="67" t="s">
         <v>139</v>
@@ -3903,7 +3903,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F40" s="67" t="s">
         <v>139</v>
@@ -3937,7 +3937,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F41" s="67" t="s">
         <v>139</v>
@@ -3971,7 +3971,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F42" s="67" t="s">
         <v>139</v>
@@ -4005,7 +4005,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F43" s="67" t="s">
         <v>139</v>
@@ -4039,7 +4039,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F44" s="67" t="s">
         <v>139</v>
@@ -4073,7 +4073,7 @@
         <v>4</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F45" s="67" t="s">
         <v>139</v>
@@ -4107,7 +4107,7 @@
         <v>4</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F46" s="67" t="s">
         <v>139</v>
@@ -4141,7 +4141,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F47" s="67" t="s">
         <v>139</v>
@@ -4175,7 +4175,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F48" s="67" t="s">
         <v>139</v>
@@ -4209,7 +4209,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F49" s="67" t="s">
         <v>139</v>
@@ -4243,7 +4243,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F50" s="67" t="s">
         <v>139</v>
@@ -4277,7 +4277,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F51" s="67" t="s">
         <v>139</v>
@@ -4311,7 +4311,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F52" s="67" t="s">
         <v>139</v>
@@ -4345,7 +4345,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F53" s="67" t="s">
         <v>139</v>
@@ -4379,7 +4379,7 @@
         <v>4</v>
       </c>
       <c r="E54" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F54" s="67" t="s">
         <v>139</v>
@@ -4413,7 +4413,7 @@
         <v>4</v>
       </c>
       <c r="E55" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F55" s="67" t="s">
         <v>139</v>
@@ -4447,7 +4447,7 @@
         <v>4</v>
       </c>
       <c r="E56" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F56" s="67" t="s">
         <v>139</v>
@@ -4481,7 +4481,7 @@
         <v>4</v>
       </c>
       <c r="E57" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F57" s="67" t="s">
         <v>139</v>
@@ -4515,7 +4515,7 @@
         <v>4</v>
       </c>
       <c r="E58" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F58" s="67" t="s">
         <v>139</v>
@@ -4549,7 +4549,7 @@
         <v>4</v>
       </c>
       <c r="E59" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F59" s="67" t="s">
         <v>139</v>
@@ -4601,7 +4601,7 @@
         <v>4</v>
       </c>
       <c r="E61" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F61" s="66" t="s">
         <v>140</v>
@@ -4635,7 +4635,7 @@
         <v>4</v>
       </c>
       <c r="E62" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F62" s="66" t="s">
         <v>140</v>
@@ -4669,7 +4669,7 @@
         <v>4</v>
       </c>
       <c r="E63" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F63" s="66" t="s">
         <v>140</v>
@@ -4703,7 +4703,7 @@
         <v>4</v>
       </c>
       <c r="E64" s="26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F64" s="66" t="s">
         <v>140</v>
@@ -4755,7 +4755,7 @@
         <v>4</v>
       </c>
       <c r="E66" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F66" s="66" t="s">
         <v>143</v>
@@ -4789,7 +4789,7 @@
         <v>4</v>
       </c>
       <c r="E67" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F67" s="66" t="s">
         <v>143</v>
@@ -4823,7 +4823,7 @@
         <v>4</v>
       </c>
       <c r="E68" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F68" s="66" t="s">
         <v>143</v>
@@ -4857,7 +4857,7 @@
         <v>4</v>
       </c>
       <c r="E69" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F69" s="66" t="s">
         <v>143</v>
@@ -4891,7 +4891,7 @@
         <v>4</v>
       </c>
       <c r="E70" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F70" s="66" t="s">
         <v>143</v>
@@ -4925,7 +4925,7 @@
         <v>4</v>
       </c>
       <c r="E71" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F71" s="66" t="s">
         <v>143</v>
@@ -4959,7 +4959,7 @@
         <v>4</v>
       </c>
       <c r="E72" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F72" s="66" t="s">
         <v>143</v>
@@ -4995,7 +4995,7 @@
         <v>4</v>
       </c>
       <c r="E73" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F73" s="66" t="s">
         <v>143</v>
@@ -5031,7 +5031,7 @@
         <v>4</v>
       </c>
       <c r="E74" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F74" s="66" t="s">
         <v>143</v>
@@ -5067,7 +5067,7 @@
         <v>4</v>
       </c>
       <c r="E75" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F75" s="66" t="s">
         <v>143</v>
@@ -5121,7 +5121,7 @@
         <v>4</v>
       </c>
       <c r="E77" s="80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F77" s="66" t="s">
         <v>144</v>
@@ -5157,7 +5157,7 @@
         <v>4</v>
       </c>
       <c r="E78" s="80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F78" s="66" t="s">
         <v>144</v>
@@ -5193,7 +5193,7 @@
         <v>4</v>
       </c>
       <c r="E79" s="80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F79" s="66" t="s">
         <v>144</v>
@@ -5227,7 +5227,7 @@
         <v>4</v>
       </c>
       <c r="E80" s="80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F80" s="66" t="s">
         <v>144</v>
@@ -5261,7 +5261,7 @@
         <v>4</v>
       </c>
       <c r="E81" s="80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F81" s="66" t="s">
         <v>144</v>
@@ -5295,7 +5295,7 @@
         <v>4</v>
       </c>
       <c r="E82" s="80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F82" s="66" t="s">
         <v>144</v>
@@ -5329,7 +5329,7 @@
         <v>4</v>
       </c>
       <c r="E83" s="80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F83" s="66" t="s">
         <v>144</v>
@@ -5381,7 +5381,7 @@
         <v>4</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F85" s="67" t="s">
         <v>149</v>
@@ -5415,7 +5415,7 @@
         <v>4</v>
       </c>
       <c r="E86" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F86" s="67" t="s">
         <v>149</v>
@@ -5449,7 +5449,7 @@
         <v>4</v>
       </c>
       <c r="E87" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F87" s="67" t="s">
         <v>149</v>
@@ -5483,7 +5483,7 @@
         <v>4</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F88" s="67" t="s">
         <v>149</v>
@@ -5517,7 +5517,7 @@
         <v>4</v>
       </c>
       <c r="E89" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F89" s="67" t="s">
         <v>149</v>
@@ -5551,7 +5551,7 @@
         <v>4</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F90" s="67" t="s">
         <v>149</v>
@@ -5585,7 +5585,7 @@
         <v>4</v>
       </c>
       <c r="E91" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F91" s="67" t="s">
         <v>149</v>
@@ -5619,7 +5619,7 @@
         <v>4</v>
       </c>
       <c r="E92" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F92" s="67" t="s">
         <v>149</v>
@@ -5671,7 +5671,7 @@
         <v>4</v>
       </c>
       <c r="E94" s="80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F94" s="66" t="s">
         <v>155</v>
@@ -5705,7 +5705,7 @@
         <v>4</v>
       </c>
       <c r="E95" s="80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F95" s="66" t="s">
         <v>155</v>
@@ -5739,7 +5739,7 @@
         <v>4</v>
       </c>
       <c r="E96" s="80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F96" s="66" t="s">
         <v>155</v>
@@ -5773,7 +5773,7 @@
         <v>4</v>
       </c>
       <c r="E97" s="80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F97" s="66" t="s">
         <v>155</v>
@@ -5807,7 +5807,7 @@
         <v>4</v>
       </c>
       <c r="E98" s="80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F98" s="66" t="s">
         <v>155</v>
@@ -5841,7 +5841,7 @@
         <v>4</v>
       </c>
       <c r="E99" s="80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F99" s="66" t="s">
         <v>155</v>
@@ -5875,7 +5875,7 @@
         <v>4</v>
       </c>
       <c r="E100" s="80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F100" s="79" t="s">
         <v>155</v>
@@ -5929,7 +5929,7 @@
         <v>4</v>
       </c>
       <c r="E102" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F102" s="66" t="s">
         <v>156</v>
@@ -5963,7 +5963,7 @@
         <v>4</v>
       </c>
       <c r="E103" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F103" s="66" t="s">
         <v>156</v>
@@ -5997,7 +5997,7 @@
         <v>4</v>
       </c>
       <c r="E104" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F104" s="66" t="s">
         <v>156</v>
@@ -6049,7 +6049,7 @@
         <v>4</v>
       </c>
       <c r="E106" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F106" s="67" t="s">
         <v>159</v>
@@ -6083,7 +6083,7 @@
         <v>4</v>
       </c>
       <c r="E107" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F107" s="67" t="s">
         <v>159</v>

</xml_diff>